<commit_message>
fixed harvester column in rnasamples -- holly added S.GISH to harvester in bioSamples
</commit_message>
<xml_diff>
--- a/old_database/crypto/rnaSample/rnaSample_0629_0618.xlsx
+++ b/old_database/crypto/rnaSample/rnaSample_0629_0618.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="14">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">10.07.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.GISH</t>
   </si>
   <si>
     <t xml:space="preserve">Retrofitted_0629_0618</t>
@@ -68,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -98,13 +101,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,16 +152,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -193,12 +185,14 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -220,7 +214,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -241,13 +235,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,13 +258,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,18 +281,18 @@
         <v>8</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>9</v>
@@ -307,21 +301,21 @@
         <v>4</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>9</v>
@@ -330,21 +324,21 @@
         <v>5</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>9</v>
@@ -353,21 +347,21 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>9</v>
@@ -376,21 +370,21 @@
         <v>7</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>9</v>
@@ -399,21 +393,21 @@
         <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>9</v>
@@ -422,21 +416,21 @@
         <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>9</v>
@@ -445,21 +439,21 @@
         <v>10</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>9</v>
@@ -468,16 +462,16 @@
         <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,18 +488,18 @@
         <v>8</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>9</v>
@@ -514,21 +508,21 @@
         <v>13</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>9</v>
@@ -537,16 +531,16 @@
         <v>14</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>10</v>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,18 +557,18 @@
         <v>8</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>9</v>
@@ -583,16 +577,16 @@
         <v>16</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,18 +603,18 @@
         <v>8</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>9</v>
@@ -629,21 +623,21 @@
         <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>9</v>
@@ -652,21 +646,21 @@
         <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>19</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>9</v>
@@ -675,21 +669,21 @@
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>9</v>
@@ -698,21 +692,21 @@
         <v>21</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>21</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>9</v>
@@ -721,21 +715,21 @@
         <v>22</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>22</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>9</v>
@@ -744,21 +738,21 @@
         <v>23</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>23</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>9</v>
@@ -767,16 +761,16 @@
         <v>24</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>24</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>